<commit_message>
team sheets separated per assignment requirements
</commit_message>
<xml_diff>
--- a/docs/Team Task Sheet_(Web Enterprise_Database Design and Implementation_Cohort 1_Team11).xlsx
+++ b/docs/Team Task Sheet_(Web Enterprise_Database Design and Implementation_Cohort 1_Team11).xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="R+U5S2SxM4m5pW8e8hdZIn9QwTl/A3qpRJje5ry6sJg="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="yRkZXk3HNR6R7/XutPqjoEkZpI3CXcOp2RQMrER+sYM="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>Please ensure this tracking sheet is completed as a group, as it will be used to monitor your individual participation within the team.</t>
   </si>
@@ -33,7 +33,7 @@
     <t>Teta Butera Nelly</t>
   </si>
   <si>
-    <t>Every team member has a dynamic role and their responsibilities are carried out through completing their assigned tasks as distributed on our scrum board</t>
+    <t>ERD Drawing for the rest of the assignments and README updates</t>
   </si>
   <si>
     <t>t.nelly@alustudent.com</t>
@@ -42,10 +42,16 @@
     <t>Ingabe Mbayire Melyssa</t>
   </si>
   <si>
+    <t>Incharge of Scrum Board Updates</t>
+  </si>
+  <si>
     <t>m.mbayire@alustudent.com</t>
   </si>
   <si>
     <t>Bonheur MURENZI</t>
+  </si>
+  <si>
+    <t>SQL DB implementation</t>
   </si>
   <si>
     <t>m.bonheur@alustudent.com</t>
@@ -73,10 +79,10 @@
     <t>Comments</t>
   </si>
   <si>
-    <t xml:space="preserve">setup github team repository </t>
+    <t>Entity relationship diagram and ERD Documentation in (erd_diagram.pdf)</t>
   </si>
   <si>
-    <t>15th January 2026</t>
+    <t>26th January 2026</t>
   </si>
   <si>
     <t>Completed</t>
@@ -85,37 +91,10 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Set up Scrum Board using Jira</t>
+    <t>SQL Database Implementation and Sample Queries Documentation</t>
   </si>
   <si>
-    <t>Drawing a high-level draft system architecture diagram using Miro</t>
-  </si>
-  <si>
-    <t>Research MoMo SMS XML structure</t>
-  </si>
-  <si>
-    <t>25th January 2026</t>
-  </si>
-  <si>
-    <t>In progress</t>
-  </si>
-  <si>
-    <t>Building and securing a REST API</t>
-  </si>
-  <si>
-    <t>26th January 2026</t>
-  </si>
-  <si>
-    <t>Not started</t>
-  </si>
-  <si>
-    <t>Entity relationship diagram</t>
-  </si>
-  <si>
-    <t>SQL Database Implementation</t>
-  </si>
-  <si>
-    <t>JSON Data Modeling</t>
+    <t>JSON Data Modeling and Scrum Board Updates</t>
   </si>
   <si>
     <t>UPDATE TEAM SHEET</t>
@@ -142,43 +121,16 @@
     <t>Next Steps</t>
   </si>
   <si>
-    <t>13th January 2026</t>
+    <t>22th January 2026</t>
   </si>
   <si>
-    <t>1. Welcome &amp; Introductions 2.Assignment 3.OverviewUnderstanding the Task</t>
-  </si>
-  <si>
-    <t>David Neza</t>
+    <t xml:space="preserve">1. Review progress from the previous meeting 2. Finalize database requirements and assumptions 3. Discuss and plan ERD design 4.Plan ERD documentation </t>
   </si>
   <si>
     <t xml:space="preserve">Teta Nelly
 Melyssa Mbayire
 Bonheur MURENZI
 </t>
-  </si>
-  <si>
-    <t>In the first meeting, we discuss the assignment requirements, including objectives, deliverables, and deadlines. we  share initial ideas, agree on the scope of work, and decide how tasks will be divided based on individual strengths.we also set a timeline, choose communication tools, and confirm next steps and the next meeting date.</t>
-  </si>
-  <si>
-    <t>1.assign tasks to each team member                         2.agree on internal deadlines</t>
-  </si>
-  <si>
-    <t>1. Review progress since the last meeting  2. Individual updates on assigned tasks     3. Discussion of challenges or issues        4. Feedback and improvements                 5. Confirm next steps and next meeting date</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>we discuss the progress made by each member and check whether tasks are on schedule. Any problems or difficulties faced during the work addressed, and feedback shared to improve the quality of the assignment. we refine ideas or content if needed, update deadlines, and clearly define the next set of tasks before ending the meeting.</t>
-  </si>
-  <si>
-    <t>After the meeting, each team member should revise or continue their assigned work based on the feedback received. Outstanding tasks should be completed according to the updated timeline and uploaded to the shared workspace.</t>
-  </si>
-  <si>
-    <t>22th January 2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Review progress from the previous meeting 2. Finalize database requirements and assumptions 3. Discuss and plan ERD design 4.Plan ERD documentation </t>
   </si>
   <si>
     <t xml:space="preserve">We discuss the current progress and confirm the finalized database requirements. The ERD structure, including entities, relationships, and constraints, will be reviewed and agreed upon. </t>
@@ -200,10 +152,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-  </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -236,12 +185,11 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="10.0"/>
-      <color theme="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -251,11 +199,6 @@
       <name val="Times New Roman"/>
     </font>
     <font/>
-    <font>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -277,7 +220,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border/>
     <border>
       <left/>
@@ -295,11 +238,6 @@
       <bottom/>
     </border>
     <border>
-      <right/>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -308,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -323,33 +261,23 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
@@ -575,7 +503,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="21.13"/>
-    <col customWidth="1" min="2" max="2" width="42.0"/>
+    <col customWidth="1" min="2" max="2" width="54.5"/>
     <col customWidth="1" min="3" max="3" width="27.25"/>
     <col customWidth="1" min="4" max="4" width="28.25"/>
     <col customWidth="1" min="5" max="5" width="25.88"/>
@@ -641,7 +569,7 @@
       <c r="Y2" s="2"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -674,11 +602,14 @@
       <c r="Y3" s="2"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="C4" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -705,10 +636,13 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -787,14 +721,14 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
-      <c r="G8" s="10"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -815,24 +749,24 @@
       <c r="Y8" s="2"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="11" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>17</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -855,20 +789,20 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="2"/>
-      <c r="B10" s="2" t="s">
-        <v>18</v>
+      <c r="B10" s="5" t="s">
+        <v>20</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>19</v>
+      <c r="D10" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -892,20 +826,20 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="2"/>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="F11" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -929,20 +863,20 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="2"/>
-      <c r="B12" s="2" t="s">
-        <v>23</v>
+      <c r="B12" s="5" t="s">
+        <v>25</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>4</v>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -967,16 +901,19 @@
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>26</v>
+      <c r="E13" s="2" t="s">
+        <v>22</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>21</v>
+      <c r="F13" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1000,21 +937,11 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="2"/>
-      <c r="B14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -1037,21 +964,11 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="2"/>
-      <c r="B15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -1074,21 +991,11 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="2"/>
-      <c r="B16" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1111,21 +1018,11 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -1147,23 +1044,15 @@
       <c r="Y17" s="2"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="2"/>
-      <c r="B18" s="5" t="s">
-        <v>33</v>
+      <c r="A18" s="8" t="s">
+        <v>27</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G18" s="2"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -1184,13 +1073,25 @@
       <c r="Y18" s="2"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="A19" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="10"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1210,13 +1111,23 @@
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+    <row r="20" ht="72.75" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="D20" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -1237,13 +1148,23 @@
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+    <row r="21" ht="74.25" customHeight="1">
+      <c r="A21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="D21" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>41</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1292,15 +1213,13 @@
       <c r="Y22" s="2"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="10"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -1321,25 +1240,13 @@
       <c r="Y23" s="2"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G24" s="11"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -1360,24 +1267,12 @@
       <c r="Y24" s="2"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>46</v>
-      </c>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -1399,24 +1294,12 @@
       <c r="Y25" s="2"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>50</v>
-      </c>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -1438,22 +1321,12 @@
       <c r="Y26" s="2"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>54</v>
-      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -1475,22 +1348,12 @@
       <c r="Y27" s="2"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>55</v>
-      </c>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="F28" s="17" t="s">
-        <v>57</v>
-      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -1540,7 +1403,7 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="2"/>
-      <c r="B30" s="5"/>
+      <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1593,8 +1456,8 @@
       <c r="Y31" s="2"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="2"/>
-      <c r="B32" s="5"/>
+      <c r="A32" s="14"/>
+      <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1620,7 +1483,7 @@
       <c r="Y32" s="2"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="2"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1647,8 +1510,8 @@
       <c r="Y33" s="2"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="2"/>
-      <c r="B34" s="5"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -1674,7 +1537,7 @@
       <c r="Y34" s="2"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="2"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1702,7 +1565,7 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="2"/>
-      <c r="B36" s="5"/>
+      <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1728,7 +1591,7 @@
       <c r="Y36" s="2"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="2"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -1755,8 +1618,8 @@
       <c r="Y37" s="2"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="2"/>
-      <c r="B38" s="5"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -1782,7 +1645,7 @@
       <c r="Y38" s="2"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="18"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -1809,8 +1672,8 @@
       <c r="Y39" s="2"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="19"/>
-      <c r="B40" s="5"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -1836,7 +1699,7 @@
       <c r="Y40" s="2"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="19"/>
+      <c r="A41" s="15"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1863,7 +1726,7 @@
       <c r="Y41" s="2"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="19"/>
+      <c r="A42" s="15"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -1890,7 +1753,7 @@
       <c r="Y42" s="2"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="2"/>
+      <c r="A43" s="15"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -1917,7 +1780,7 @@
       <c r="Y43" s="2"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="19"/>
+      <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -1944,7 +1807,7 @@
       <c r="Y44" s="2"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="19"/>
+      <c r="A45" s="15"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -1971,7 +1834,7 @@
       <c r="Y45" s="2"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="19"/>
+      <c r="A46" s="15"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -1998,7 +1861,7 @@
       <c r="Y46" s="2"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="19"/>
+      <c r="A47" s="15"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -2025,7 +1888,7 @@
       <c r="Y47" s="2"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="19"/>
+      <c r="A48" s="15"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -2052,7 +1915,7 @@
       <c r="Y48" s="2"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="19"/>
+      <c r="A49" s="15"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -2079,7 +1942,7 @@
       <c r="Y49" s="2"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="19"/>
+      <c r="A50" s="15"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -2106,7 +1969,7 @@
       <c r="Y50" s="2"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="2"/>
+      <c r="A51" s="15"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -2133,7 +1996,7 @@
       <c r="Y51" s="2"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="19"/>
+      <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -2160,7 +2023,7 @@
       <c r="Y52" s="2"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="19"/>
+      <c r="A53" s="15"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -2187,7 +2050,7 @@
       <c r="Y53" s="2"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="19"/>
+      <c r="A54" s="15"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -2214,7 +2077,7 @@
       <c r="Y54" s="2"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="19"/>
+      <c r="A55" s="15"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -2241,7 +2104,7 @@
       <c r="Y55" s="2"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="19"/>
+      <c r="A56" s="15"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -2268,7 +2131,7 @@
       <c r="Y56" s="2"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="19"/>
+      <c r="A57" s="15"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -2295,7 +2158,7 @@
       <c r="Y57" s="2"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="19"/>
+      <c r="A58" s="15"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -2322,7 +2185,7 @@
       <c r="Y58" s="2"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="2"/>
+      <c r="A59" s="15"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -2349,7 +2212,7 @@
       <c r="Y59" s="2"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="19"/>
+      <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -2376,7 +2239,7 @@
       <c r="Y60" s="2"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="19"/>
+      <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -2403,7 +2266,7 @@
       <c r="Y61" s="2"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="19"/>
+      <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -2430,7 +2293,7 @@
       <c r="Y62" s="2"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="19"/>
+      <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -2457,7 +2320,7 @@
       <c r="Y63" s="2"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="19"/>
+      <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -2484,7 +2347,7 @@
       <c r="Y64" s="2"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="19"/>
+      <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -2511,7 +2374,7 @@
       <c r="Y65" s="2"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="19"/>
+      <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -6695,195 +6558,13 @@
       <c r="X220" s="2"/>
       <c r="Y220" s="2"/>
     </row>
-    <row r="221" ht="15.75" customHeight="1">
-      <c r="A221" s="2"/>
-      <c r="B221" s="2"/>
-      <c r="C221" s="2"/>
-      <c r="D221" s="2"/>
-      <c r="E221" s="2"/>
-      <c r="F221" s="2"/>
-      <c r="G221" s="2"/>
-      <c r="H221" s="2"/>
-      <c r="I221" s="2"/>
-      <c r="J221" s="2"/>
-      <c r="K221" s="2"/>
-      <c r="L221" s="2"/>
-      <c r="M221" s="2"/>
-      <c r="N221" s="2"/>
-      <c r="O221" s="2"/>
-      <c r="P221" s="2"/>
-      <c r="Q221" s="2"/>
-      <c r="R221" s="2"/>
-      <c r="S221" s="2"/>
-      <c r="T221" s="2"/>
-      <c r="U221" s="2"/>
-      <c r="V221" s="2"/>
-      <c r="W221" s="2"/>
-      <c r="X221" s="2"/>
-      <c r="Y221" s="2"/>
-    </row>
-    <row r="222" ht="15.75" customHeight="1">
-      <c r="A222" s="2"/>
-      <c r="B222" s="2"/>
-      <c r="C222" s="2"/>
-      <c r="D222" s="2"/>
-      <c r="E222" s="2"/>
-      <c r="F222" s="2"/>
-      <c r="G222" s="2"/>
-      <c r="H222" s="2"/>
-      <c r="I222" s="2"/>
-      <c r="J222" s="2"/>
-      <c r="K222" s="2"/>
-      <c r="L222" s="2"/>
-      <c r="M222" s="2"/>
-      <c r="N222" s="2"/>
-      <c r="O222" s="2"/>
-      <c r="P222" s="2"/>
-      <c r="Q222" s="2"/>
-      <c r="R222" s="2"/>
-      <c r="S222" s="2"/>
-      <c r="T222" s="2"/>
-      <c r="U222" s="2"/>
-      <c r="V222" s="2"/>
-      <c r="W222" s="2"/>
-      <c r="X222" s="2"/>
-      <c r="Y222" s="2"/>
-    </row>
-    <row r="223" ht="15.75" customHeight="1">
-      <c r="A223" s="2"/>
-      <c r="B223" s="2"/>
-      <c r="C223" s="2"/>
-      <c r="D223" s="2"/>
-      <c r="E223" s="2"/>
-      <c r="F223" s="2"/>
-      <c r="G223" s="2"/>
-      <c r="H223" s="2"/>
-      <c r="I223" s="2"/>
-      <c r="J223" s="2"/>
-      <c r="K223" s="2"/>
-      <c r="L223" s="2"/>
-      <c r="M223" s="2"/>
-      <c r="N223" s="2"/>
-      <c r="O223" s="2"/>
-      <c r="P223" s="2"/>
-      <c r="Q223" s="2"/>
-      <c r="R223" s="2"/>
-      <c r="S223" s="2"/>
-      <c r="T223" s="2"/>
-      <c r="U223" s="2"/>
-      <c r="V223" s="2"/>
-      <c r="W223" s="2"/>
-      <c r="X223" s="2"/>
-      <c r="Y223" s="2"/>
-    </row>
-    <row r="224" ht="15.75" customHeight="1">
-      <c r="A224" s="2"/>
-      <c r="B224" s="2"/>
-      <c r="C224" s="2"/>
-      <c r="D224" s="2"/>
-      <c r="E224" s="2"/>
-      <c r="F224" s="2"/>
-      <c r="G224" s="2"/>
-      <c r="H224" s="2"/>
-      <c r="I224" s="2"/>
-      <c r="J224" s="2"/>
-      <c r="K224" s="2"/>
-      <c r="L224" s="2"/>
-      <c r="M224" s="2"/>
-      <c r="N224" s="2"/>
-      <c r="O224" s="2"/>
-      <c r="P224" s="2"/>
-      <c r="Q224" s="2"/>
-      <c r="R224" s="2"/>
-      <c r="S224" s="2"/>
-      <c r="T224" s="2"/>
-      <c r="U224" s="2"/>
-      <c r="V224" s="2"/>
-      <c r="W224" s="2"/>
-      <c r="X224" s="2"/>
-      <c r="Y224" s="2"/>
-    </row>
-    <row r="225" ht="15.75" customHeight="1">
-      <c r="A225" s="2"/>
-      <c r="B225" s="2"/>
-      <c r="C225" s="2"/>
-      <c r="D225" s="2"/>
-      <c r="E225" s="2"/>
-      <c r="F225" s="2"/>
-      <c r="G225" s="2"/>
-      <c r="H225" s="2"/>
-      <c r="I225" s="2"/>
-      <c r="J225" s="2"/>
-      <c r="K225" s="2"/>
-      <c r="L225" s="2"/>
-      <c r="M225" s="2"/>
-      <c r="N225" s="2"/>
-      <c r="O225" s="2"/>
-      <c r="P225" s="2"/>
-      <c r="Q225" s="2"/>
-      <c r="R225" s="2"/>
-      <c r="S225" s="2"/>
-      <c r="T225" s="2"/>
-      <c r="U225" s="2"/>
-      <c r="V225" s="2"/>
-      <c r="W225" s="2"/>
-      <c r="X225" s="2"/>
-      <c r="Y225" s="2"/>
-    </row>
-    <row r="226" ht="15.75" customHeight="1">
-      <c r="A226" s="2"/>
-      <c r="B226" s="2"/>
-      <c r="C226" s="2"/>
-      <c r="D226" s="2"/>
-      <c r="E226" s="2"/>
-      <c r="F226" s="2"/>
-      <c r="G226" s="2"/>
-      <c r="H226" s="2"/>
-      <c r="I226" s="2"/>
-      <c r="J226" s="2"/>
-      <c r="K226" s="2"/>
-      <c r="L226" s="2"/>
-      <c r="M226" s="2"/>
-      <c r="N226" s="2"/>
-      <c r="O226" s="2"/>
-      <c r="P226" s="2"/>
-      <c r="Q226" s="2"/>
-      <c r="R226" s="2"/>
-      <c r="S226" s="2"/>
-      <c r="T226" s="2"/>
-      <c r="U226" s="2"/>
-      <c r="V226" s="2"/>
-      <c r="W226" s="2"/>
-      <c r="X226" s="2"/>
-      <c r="Y226" s="2"/>
-    </row>
-    <row r="227" ht="15.75" customHeight="1">
-      <c r="A227" s="2"/>
-      <c r="B227" s="2"/>
-      <c r="C227" s="2"/>
-      <c r="D227" s="2"/>
-      <c r="E227" s="2"/>
-      <c r="F227" s="2"/>
-      <c r="G227" s="2"/>
-      <c r="H227" s="2"/>
-      <c r="I227" s="2"/>
-      <c r="J227" s="2"/>
-      <c r="K227" s="2"/>
-      <c r="L227" s="2"/>
-      <c r="M227" s="2"/>
-      <c r="N227" s="2"/>
-      <c r="O227" s="2"/>
-      <c r="P227" s="2"/>
-      <c r="Q227" s="2"/>
-      <c r="R227" s="2"/>
-      <c r="S227" s="2"/>
-      <c r="T227" s="2"/>
-      <c r="U227" s="2"/>
-      <c r="V227" s="2"/>
-      <c r="W227" s="2"/>
-      <c r="X227" s="2"/>
-      <c r="Y227" s="2"/>
-    </row>
+    <row r="221" ht="15.75" customHeight="1"/>
+    <row r="222" ht="15.75" customHeight="1"/>
+    <row r="223" ht="15.75" customHeight="1"/>
+    <row r="224" ht="15.75" customHeight="1"/>
+    <row r="225" ht="15.75" customHeight="1"/>
+    <row r="226" ht="15.75" customHeight="1"/>
+    <row r="227" ht="15.75" customHeight="1"/>
     <row r="228" ht="15.75" customHeight="1"/>
     <row r="229" ht="15.75" customHeight="1"/>
     <row r="230" ht="15.75" customHeight="1"/>
@@ -7654,25 +7335,17 @@
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
-    <row r="1001" ht="15.75" customHeight="1"/>
-    <row r="1002" ht="15.75" customHeight="1"/>
-    <row r="1003" ht="15.75" customHeight="1"/>
-    <row r="1004" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="A18:G18"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E10:E18">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E10:E13">
       <formula1>"Not started,In progress,Completed,Did not participate"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F10:F18">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F10:F13">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>